<commit_message>
data updated on 2025-05-28 11:42:34.963887
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Log" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Log" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -35,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -43,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,25 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,17 +434,25 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Last Updated</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>2025-05-28 10:53:40</t>
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-05-28 11:42:34</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-05-28 11:43:47.219153
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,11 +439,6 @@
           <t>Last Updated</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>2025-05-28 10:53:40</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -451,7 +446,13 @@
           <t>2025-05-28 11:42:34</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-05-28 11:43:47</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
data updated on 2025-06-20 14:57:42.106094
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -1,54 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M.HARISH\PycharmProjects\Chile_Ley_del_Lobby_Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8926AFB6-777A-4485-B539-5848AB31DE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Log" sheetId="1" r:id="rId1"/>
+    <sheet name="Log" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Last Updated</t>
-  </si>
-  <si>
-    <t>2025-05-28 11:42:34</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -63,44 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -388,31 +424,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Last Updated</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-05-28 11:42:34</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>45820.488738425927</v>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45820.48873842593</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-06-20 14:57:42</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data updated on 2025-06-30 16:42:36.128868
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Log" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Log" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,6 +463,13 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-06-30 16:42:36</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-07-08 22:15:29.269774
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,6 +470,13 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-07-08 22:15:29</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-07-14 18:18:00.762406
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,13 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-07-14 18:18:00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-07-23 10:16:42.476491
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,13 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-07-23 10:16:42</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-08-04 17:46:01.343289
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,6 +498,13 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-08-04 17:46:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-08-12 15:00:07.562455
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +505,13 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-08-12 15:00:07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-08-25 22:44:36.110181
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,6 +512,13 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-08-25 22:44:36</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-09-03 21:46:40.570945
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,13 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-09-03 21:46:40</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-09-08 10:27:25.605769
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +526,13 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-09-08 10:27:25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-09-19 10:24:37.647036
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,6 +533,13 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-09-19 10:24:37</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-09-23 10:45:16.296180
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,6 +540,13 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-09-23 10:45:16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-10-07 11:22:47.128270
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,6 +547,13 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-10-07 11:22:47</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-10-07 11:23:05.961937
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,13 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-10-07 11:23:05</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-10-14 13:50:10.027121
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +561,13 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-10-14 13:50:10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-10-14 21:10:42.631129
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,6 +568,13 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-10-14 21:10:42</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-10-15 10:53:06.889549
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,6 +575,13 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-10-15 10:53:06</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-10-15 12:41:06.659271
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,6 +582,13 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-10-15 12:41:06</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-10-15 20:50:49.932325
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,6 +589,13 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-10-15 20:50:49</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-11-04 22:38:48.982564
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,6 +603,13 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-11-04 22:38:48</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2025-11-15 14:07:47.290739
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,6 +610,13 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-11-15 14:07:47</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data updated on 2026-01-12 14:57:58.709078
</commit_message>
<xml_diff>
--- a/update_log.xlsx
+++ b/update_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -624,6 +624,13 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-01-12 14:57:58</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>